<commit_message>
deleted:    ../../.classpath 	deleted:    ../../.project 	deleted:    ../../.settings/org.eclipse.core.resources.prefs 	deleted:    ../../.settings/org.eclipse.jdt.core.prefs 	deleted:    ../../.settings/org.eclipse.m2e.core.prefs 	modified:   ../../NaukriUpdate/test data/data1.xlsx 	deleted:    ../../hai.txt 	deleted:    ../../pom.xml 	deleted:    ../../src/main/java/naukri/update/App.java 	deleted:    ../../src/test/java/naukri/update/AppTest.java 	deleted:    ../../target/classes/naukri/update/App.class 	deleted:    ../../target/test-classes/naukri/update/AppTest.class
</commit_message>
<xml_diff>
--- a/NaukriUpdate/test data/data1.xlsx
+++ b/NaukriUpdate/test data/data1.xlsx
@@ -14,73 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
-  <si>
-    <t>1014401312hari</t>
-  </si>
-  <si>
-    <t>harivardhan.qa@gmail.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>D:\\hari vardhan\\Resume.doc</t>
-  </si>
-  <si>
-    <t>Wed May 25 22:55:33 IST 2016</t>
   </si>
   <si>
     <t>Resume Uploaded Successfully</t>
   </si>
   <si>
-    <t>Wed May 25 23:08:16 IST 2016</t>
+    <t>Tue May 31 09:18:27 IST 2016</t>
   </si>
   <si>
-    <t>Wed May 25 23:09:39 IST 2016</t>
+    <t>xyz</t>
   </si>
   <si>
-    <t>Wed May 25 23:14:45 IST 2016</t>
-  </si>
-  <si>
-    <t>Wed May 25 23:15:26 IST 2016</t>
-  </si>
-  <si>
-    <t>Wed May 25 23:23:32 IST 2016</t>
-  </si>
-  <si>
-    <t>Wed May 25 23:25:21 IST 2016</t>
-  </si>
-  <si>
-    <t>Wed May 25 23:26:06 IST 2016</t>
-  </si>
-  <si>
-    <t>Wed May 25 23:29:00 IST 2016</t>
-  </si>
-  <si>
-    <t>Wed May 25 23:30:50 IST 2016</t>
-  </si>
-  <si>
-    <t>Wed May 25 23:50:34 IST 2016</t>
-  </si>
-  <si>
-    <t>Thu May 26 07:50:44 IST 2016</t>
-  </si>
-  <si>
-    <t>Thu May 26 08:50:32 IST 2016</t>
-  </si>
-  <si>
-    <t>Thu May 26 22:50:43 IST 2016</t>
-  </si>
-  <si>
-    <t>Mon May 30 08:51:24 IST 2016</t>
-  </si>
-  <si>
-    <t>Tue May 31 09:18:27 IST 2016</t>
+    <t>xyz.qa@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,33 +384,33 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="36.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>